<commit_message>
Actualización automática desde Streamlit
</commit_message>
<xml_diff>
--- a/data_base.xlsx
+++ b/data_base.xlsx
@@ -2347,7 +2347,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B96" t="n">
         <v>15</v>
@@ -2359,7 +2359,7 @@
         <v>50</v>
       </c>
       <c r="E96" t="n">
-        <v>84.62</v>
+        <v>84.75</v>
       </c>
       <c r="F96" t="n">
         <v>10201</v>

</xml_diff>